<commit_message>
Made that things do not trip in case of an Exception
</commit_message>
<xml_diff>
--- a/src/module_1/p6_test results.xlsx
+++ b/src/module_1/p6_test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/faf89f17094f69d9/_School/2024_TU Delft Bsc EE/2025-2026/Q2_EE2L1/Project/src/module_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8E6FD56-DB3F-4088-9C7F-52AA87C6C69E}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C58E43A-D9B1-4DAE-AFD2-2F6088ED7993}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="11640" windowWidth="28485" windowHeight="5430" xr2:uid="{27495DE4-06DE-42D5-9603-5AE5B78F0026}"/>
+    <workbookView xWindow="16410" yWindow="8925" windowWidth="28485" windowHeight="5430" xr2:uid="{27495DE4-06DE-42D5-9603-5AE5B78F0026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,6 +835,33 @@
         <f t="shared" ref="K4:K26" si="5">R4</f>
         <v>0</v>
       </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -843,6 +870,15 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" s="1">
+        <v>104</v>
+      </c>
+      <c r="D5" s="1">
+        <v>103</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -866,6 +902,33 @@
       <c r="K5" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel updated something, i do not know what
</commit_message>
<xml_diff>
--- a/src/module_1/p6_test results.xlsx
+++ b/src/module_1/p6_test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/faf89f17094f69d9/_School/2024_TU Delft Bsc EE/2025-2026/Q2_EE2L1/Project/src/module_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="464" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F61E36C-A305-41D9-9267-5D2862A01F48}"/>
+  <xr:revisionPtr revIDLastSave="476" documentId="8_{FF6D4E3F-F320-4EC6-AC2B-1AEDDC2D4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE9B4328-7274-431E-971D-FBE249B4B4CC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{27495DE4-06DE-42D5-9603-5AE5B78F0026}"/>
   </bookViews>
@@ -1664,10 +1664,10 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,6 +3289,15 @@
       <c r="B26" t="s">
         <v>29</v>
       </c>
+      <c r="C26" s="1">
+        <v>113</v>
+      </c>
+      <c r="D26" s="1">
+        <v>112</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
       <c r="F26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3311,6 +3320,33 @@
       </c>
       <c r="K26" s="2">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>0</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>